<commit_message>
import des notes et l'affichage de tous les etudiants
</commit_message>
<xml_diff>
--- a/projetASP/ExcelFiles/EtudiantExemple.xlsx
+++ b/projetASP/ExcelFiles/EtudiantExemple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuri/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0AEBBC5-233B-5846-9735-ED7DEE34C0BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F1908-6082-8440-AD42-1AE018D7B0B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="24000" xr2:uid="{48A56E2D-C0E2-E540-89C2-38A4DBCE18F6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21940" xr2:uid="{48A56E2D-C0E2-E540-89C2-38A4DBCE18F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="130">
   <si>
     <t>nom</t>
   </si>
@@ -81,44 +81,353 @@
     <t>lieu de naissance</t>
   </si>
   <si>
-    <t>hakik</t>
-  </si>
-  <si>
-    <t>ayoub</t>
-  </si>
-  <si>
-    <t>scotish</t>
-  </si>
-  <si>
-    <t>hh1hh1</t>
-  </si>
-  <si>
-    <t>1hh1hh</t>
-  </si>
-  <si>
-    <t>ayoub@gmail.com</t>
-  </si>
-  <si>
-    <t>adress exampl,48</t>
-  </si>
-  <si>
-    <t>alabama</t>
-  </si>
-  <si>
-    <t>svt</t>
-  </si>
-  <si>
-    <t>bien</t>
-  </si>
-  <si>
     <t>safi</t>
+  </si>
+  <si>
+    <t>ghita@gmail.com</t>
+  </si>
+  <si>
+    <t>exam adress</t>
+  </si>
+  <si>
+    <t>amabala</t>
+  </si>
+  <si>
+    <t>maths</t>
+  </si>
+  <si>
+    <t>triiibien</t>
+  </si>
+  <si>
+    <t>fwwf</t>
+  </si>
+  <si>
+    <t>fwf</t>
+  </si>
+  <si>
+    <t>wg</t>
+  </si>
+  <si>
+    <t>gtgwgg</t>
+  </si>
+  <si>
+    <t>wgwg</t>
+  </si>
+  <si>
+    <t>wryu</t>
+  </si>
+  <si>
+    <t>ou</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>uolulu</t>
+  </si>
+  <si>
+    <t>luluo</t>
+  </si>
+  <si>
+    <t>9qdq</t>
+  </si>
+  <si>
+    <t>fwrrgr</t>
+  </si>
+  <si>
+    <t>accac</t>
+  </si>
+  <si>
+    <t>iluulul</t>
+  </si>
+  <si>
+    <t>jtjtj</t>
+  </si>
+  <si>
+    <t>fwwdq</t>
+  </si>
+  <si>
+    <t>acac</t>
+  </si>
+  <si>
+    <t>gtgtg</t>
+  </si>
+  <si>
+    <t>juuju</t>
+  </si>
+  <si>
+    <t>poopp</t>
+  </si>
+  <si>
+    <t>qddcw</t>
+  </si>
+  <si>
+    <t>wdwf</t>
+  </si>
+  <si>
+    <t>eeq3</t>
+  </si>
+  <si>
+    <t>3r2r</t>
+  </si>
+  <si>
+    <t>r4t4t</t>
+  </si>
+  <si>
+    <t>t3t3t</t>
+  </si>
+  <si>
+    <t>t7uu7</t>
+  </si>
+  <si>
+    <t>u7u7</t>
+  </si>
+  <si>
+    <t>i0i0i</t>
+  </si>
+  <si>
+    <t>h888</t>
+  </si>
+  <si>
+    <t>g7g7</t>
+  </si>
+  <si>
+    <t>9u9l</t>
+  </si>
+  <si>
+    <t>s4s4</t>
+  </si>
+  <si>
+    <t>f6f6</t>
+  </si>
+  <si>
+    <t>s3s3</t>
+  </si>
+  <si>
+    <t>a2a2</t>
+  </si>
+  <si>
+    <t>v5v5</t>
+  </si>
+  <si>
+    <t>c3c3</t>
+  </si>
+  <si>
+    <t>c4c4</t>
+  </si>
+  <si>
+    <t>c5</t>
+  </si>
+  <si>
+    <t>c5c7</t>
+  </si>
+  <si>
+    <t>n9n9</t>
+  </si>
+  <si>
+    <t>sqsq</t>
+  </si>
+  <si>
+    <t>xqxq</t>
+  </si>
+  <si>
+    <t>cece</t>
+  </si>
+  <si>
+    <t>caca</t>
+  </si>
+  <si>
+    <t>vava</t>
+  </si>
+  <si>
+    <t>baab</t>
+  </si>
+  <si>
+    <t>lala</t>
+  </si>
+  <si>
+    <t>yaya</t>
+  </si>
+  <si>
+    <t>uyuy</t>
+  </si>
+  <si>
+    <t>vrvr</t>
+  </si>
+  <si>
+    <t>byby</t>
+  </si>
+  <si>
+    <t>bubu</t>
+  </si>
+  <si>
+    <t>bibi</t>
+  </si>
+  <si>
+    <t>bobo</t>
+  </si>
+  <si>
+    <t>veve</t>
+  </si>
+  <si>
+    <t>vtvt</t>
+  </si>
+  <si>
+    <t>vuvu</t>
+  </si>
+  <si>
+    <t>vivi</t>
+  </si>
+  <si>
+    <t>vovo</t>
+  </si>
+  <si>
+    <t>brbr</t>
+  </si>
+  <si>
+    <t>bebe</t>
+  </si>
+  <si>
+    <t>bdbd</t>
+  </si>
+  <si>
+    <t>btgr</t>
+  </si>
+  <si>
+    <t>jhgf</t>
+  </si>
+  <si>
+    <t>ggggg</t>
+  </si>
+  <si>
+    <t>fffff</t>
+  </si>
+  <si>
+    <t>ddddd</t>
+  </si>
+  <si>
+    <t>ccccc</t>
+  </si>
+  <si>
+    <t>vvvvv</t>
+  </si>
+  <si>
+    <t>eeee</t>
+  </si>
+  <si>
+    <t>uuuuu</t>
+  </si>
+  <si>
+    <t>ttttt</t>
+  </si>
+  <si>
+    <t>kkkk</t>
+  </si>
+  <si>
+    <t>pppp</t>
+  </si>
+  <si>
+    <t>mmm</t>
+  </si>
+  <si>
+    <t>lllll</t>
+  </si>
+  <si>
+    <t>ppooo</t>
+  </si>
+  <si>
+    <t>uuyyy</t>
+  </si>
+  <si>
+    <t>ttrrr</t>
+  </si>
+  <si>
+    <t>gggfff</t>
+  </si>
+  <si>
+    <t>vvddd</t>
+  </si>
+  <si>
+    <t>nggn</t>
+  </si>
+  <si>
+    <t>httth</t>
+  </si>
+  <si>
+    <t>jyyj</t>
+  </si>
+  <si>
+    <t>rrreee</t>
+  </si>
+  <si>
+    <t>wwdd</t>
+  </si>
+  <si>
+    <t>gfds</t>
+  </si>
+  <si>
+    <t>ytre</t>
+  </si>
+  <si>
+    <t>uyth</t>
+  </si>
+  <si>
+    <t>hgfd</t>
+  </si>
+  <si>
+    <t>lkjhg</t>
+  </si>
+  <si>
+    <t>lkjhtre</t>
+  </si>
+  <si>
+    <t>nbvfd</t>
+  </si>
+  <si>
+    <t>kjhgew</t>
+  </si>
+  <si>
+    <t>fdsee</t>
+  </si>
+  <si>
+    <t>mnbvc</t>
+  </si>
+  <si>
+    <t>lkjhgff</t>
+  </si>
+  <si>
+    <t>uytrhgfd</t>
+  </si>
+  <si>
+    <t>nbvfdx</t>
+  </si>
+  <si>
+    <t>qsedf</t>
+  </si>
+  <si>
+    <t>tffyhbv</t>
+  </si>
+  <si>
+    <t>ijhgvgf</t>
+  </si>
+  <si>
+    <t>plkmuh</t>
+  </si>
+  <si>
+    <t>uhgddv</t>
+  </si>
+  <si>
+    <t>jhtrrr</t>
+  </si>
+  <si>
+    <t>tfdccc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -130,6 +439,13 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,10 +472,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -475,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{468922B8-9373-4847-B8EC-A7FD9A16BFAB}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -539,57 +857,1128 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2">
-        <v>666666</v>
-      </c>
-      <c r="H2">
-        <v>6666666</v>
-      </c>
-      <c r="I2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H2" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M2" s="3">
+        <v>16</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>127</v>
+      </c>
+      <c r="C3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" t="s">
         <v>23</v>
       </c>
-      <c r="K2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H3" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M3" s="3">
+        <v>16</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" t="s">
         <v>24</v>
       </c>
-      <c r="L2">
-        <v>2015</v>
-      </c>
-      <c r="M2">
-        <v>14</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H4" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M4" s="3">
+        <v>16</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="2">
-        <v>35661</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H5" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M5" s="3">
+        <v>16</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O5" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" t="s">
         <v>26</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H6" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M6" s="3">
+        <v>16</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O6" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B7" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H7" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M7" s="3">
+        <v>16</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>94</v>
+      </c>
+      <c r="B8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8">
+        <v>777777</v>
+      </c>
+      <c r="H8">
+        <v>777777</v>
+      </c>
+      <c r="I8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>2019</v>
+      </c>
+      <c r="M8">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
+        <v>21</v>
+      </c>
+      <c r="O8" s="2">
+        <v>37229</v>
+      </c>
+      <c r="P8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B9" t="s">
+        <v>122</v>
+      </c>
+      <c r="C9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9">
+        <v>777777</v>
+      </c>
+      <c r="H9">
+        <v>777777</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9">
+        <v>2019</v>
+      </c>
+      <c r="M9">
+        <v>16</v>
+      </c>
+      <c r="N9" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="2">
+        <v>37229</v>
+      </c>
+      <c r="P9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>96</v>
+      </c>
+      <c r="B10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G10" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H10" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L10" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M10" s="3">
+        <v>16</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B11" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H11" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M11" s="3">
+        <v>16</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B12" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G12" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H12" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L12" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M12" s="3">
+        <v>16</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H13" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M13" s="3">
+        <v>16</v>
+      </c>
+      <c r="N13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G14" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H14" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L14" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M14" s="3">
+        <v>16</v>
+      </c>
+      <c r="N14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O14" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s">
+        <v>77</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H15" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L15" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M15" s="3">
+        <v>16</v>
+      </c>
+      <c r="N15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D16" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16">
+        <v>777777</v>
+      </c>
+      <c r="H16">
+        <v>777777</v>
+      </c>
+      <c r="I16" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16">
+        <v>2019</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+      <c r="N16" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="2">
+        <v>37229</v>
+      </c>
+      <c r="P16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C17" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17">
+        <v>777777</v>
+      </c>
+      <c r="H17">
+        <v>777777</v>
+      </c>
+      <c r="I17" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17">
+        <v>2019</v>
+      </c>
+      <c r="M17">
+        <v>16</v>
+      </c>
+      <c r="N17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="2">
+        <v>37229</v>
+      </c>
+      <c r="P17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B18" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H18" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L18" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M18" s="3">
+        <v>16</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>105</v>
+      </c>
+      <c r="B19" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G19" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H19" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L19" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M19" s="3">
+        <v>16</v>
+      </c>
+      <c r="N19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>82</v>
+      </c>
+      <c r="D20" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H20" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L20" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M20" s="3">
+        <v>16</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O20" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G21" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H21" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M21" s="3">
+        <v>16</v>
+      </c>
+      <c r="N21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O21" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>108</v>
+      </c>
+      <c r="B22" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" t="s">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>42</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G22" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H22" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L22" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M22" s="3">
+        <v>16</v>
+      </c>
+      <c r="N22" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" t="s">
+        <v>110</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E23" t="s">
+        <v>87</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G23" s="3">
+        <v>777777</v>
+      </c>
+      <c r="H23" s="3">
+        <v>777777</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L23" s="3">
+        <v>2019</v>
+      </c>
+      <c r="M23" s="3">
+        <v>16</v>
+      </c>
+      <c r="N23" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="O23" s="4">
+        <v>37229</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{A661B67A-A92E-474D-806C-61DFB84FE738}"/>
+    <hyperlink ref="F2" r:id="rId1" display="mailto:ghita@gmail.com" xr:uid="{F78DEFF4-A97C-1445-AB51-A917B34128E7}"/>
+    <hyperlink ref="F3" r:id="rId2" display="mailto:ghita@gmail.com" xr:uid="{AC0AF4D1-74E7-AF41-99AB-BADD63848024}"/>
+    <hyperlink ref="F4" r:id="rId3" display="mailto:ghita@gmail.com" xr:uid="{D3C502D3-C1D2-AC4C-B6C1-C99DC82525F1}"/>
+    <hyperlink ref="F5" r:id="rId4" display="mailto:ghita@gmail.com" xr:uid="{E9DCDF33-CB4A-5349-AA2D-B79E88144E12}"/>
+    <hyperlink ref="F6" r:id="rId5" display="mailto:ghita@gmail.com" xr:uid="{A2451343-B7F5-8A43-A322-F4071970657E}"/>
+    <hyperlink ref="F7" r:id="rId6" display="mailto:ghita@gmail.com" xr:uid="{5A9E7AAC-BFE2-6A44-8DA0-BDE4A705F88E}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{5AEA7134-E39C-3E44-8E6C-5D6E035FD49C}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{2C98438E-3DB7-9A45-A312-152F5983D149}"/>
+    <hyperlink ref="F10" r:id="rId9" display="mailto:ghita@gmail.com" xr:uid="{FF90BBB4-BCE9-D548-A55F-0E502D6CA1BB}"/>
+    <hyperlink ref="F11" r:id="rId10" display="mailto:ghita@gmail.com" xr:uid="{2AA6A43D-210A-9E42-8439-B453164949DC}"/>
+    <hyperlink ref="F12" r:id="rId11" display="mailto:ghita@gmail.com" xr:uid="{A8DD5C0B-2CBE-C64D-94FA-A0D04148B8A8}"/>
+    <hyperlink ref="F13" r:id="rId12" display="mailto:ghita@gmail.com" xr:uid="{8B24B724-E3F9-BE40-9E7F-4124EEB1C5E5}"/>
+    <hyperlink ref="F14" r:id="rId13" display="mailto:ghita@gmail.com" xr:uid="{50A2BAF7-28E4-0F4D-9052-D3221C1C2ED9}"/>
+    <hyperlink ref="F15" r:id="rId14" display="mailto:ghita@gmail.com" xr:uid="{66C5A23E-346A-104B-A873-453ACE9A55E5}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{6CA9D157-27B8-F347-9723-E4254CAF53D9}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{C78F49AB-6F80-2141-B75A-8927FD78AB7E}"/>
+    <hyperlink ref="F18" r:id="rId17" display="mailto:ghita@gmail.com" xr:uid="{A16422A8-9E7F-034B-A8BE-85953BC6BB88}"/>
+    <hyperlink ref="F19" r:id="rId18" display="mailto:ghita@gmail.com" xr:uid="{DBBBBC45-B99C-2443-A772-EF28A5F21CBB}"/>
+    <hyperlink ref="F20" r:id="rId19" display="mailto:ghita@gmail.com" xr:uid="{486D2E0B-CA4A-6C43-AC18-504D9CF351B3}"/>
+    <hyperlink ref="F21" r:id="rId20" display="mailto:ghita@gmail.com" xr:uid="{DC78B358-D3EF-8049-89A5-27A314371691}"/>
+    <hyperlink ref="F22" r:id="rId21" display="mailto:ghita@gmail.com" xr:uid="{9C6FEA1F-5FBF-8B4C-A07D-5C828DF2C736}"/>
+    <hyperlink ref="F23" r:id="rId22" display="mailto:ghita@gmail.com" xr:uid="{3D249064-C010-3243-8B4F-27EF8F16105A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>